<commit_message>
alles bis auf Balkenanzeige vervollständigt
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bweina\Desktop\ZP2_SMT\Dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bweina\Desktop\zp2_smt\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -656,6 +656,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -670,20 +684,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,7 +1045,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H22" sqref="H22"/>
+      <selection pane="topRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
@@ -1061,13 +1061,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="31.5">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
@@ -1086,17 +1086,17 @@
     </row>
     <row r="2" spans="1:26" customFormat="1" ht="42" customHeight="1">
       <c r="C2" s="28"/>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="48" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" thickBot="1">
       <c r="C3" s="39"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="45"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="12">
         <v>44061</v>
       </c>
@@ -1150,10 +1150,10 @@
       <c r="Z3" s="38"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="47">
-        <v>1</v>
-      </c>
-      <c r="B4" s="49" t="s">
+      <c r="A4" s="42">
+        <v>1</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -1191,8 +1191,8 @@
       <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="48"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1228,10 +1228,10 @@
       <c r="Z5" s="22"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="47">
+      <c r="A6" s="42">
         <v>2</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1279,8 +1279,8 @@
       <c r="Z6" s="23"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="48"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1316,10 +1316,10 @@
       <c r="Z7" s="22"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="47">
+      <c r="A8" s="42">
         <v>3</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1363,8 +1363,8 @@
       <c r="Z8" s="23"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1373,15 +1373,19 @@
       </c>
       <c r="E9" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="8">
         <v>1</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1400,10 +1404,10 @@
       <c r="Z9" s="22"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="47">
+      <c r="A10" s="42">
         <v>4</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="44" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1441,8 +1445,8 @@
       <c r="Z10" s="23"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="48"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1451,13 +1455,17 @@
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -1476,10 +1484,10 @@
       <c r="Z11" s="22"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="47">
+      <c r="A12" s="42">
         <v>5</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1517,8 +1525,8 @@
       <c r="Z12" s="23"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1552,10 +1560,10 @@
       <c r="Z13" s="22"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="47">
+      <c r="A14" s="42">
         <v>6</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="44" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1593,8 +1601,8 @@
       <c r="Z14" s="23"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1628,10 +1636,10 @@
       <c r="Z15" s="22"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="47">
+      <c r="A16" s="42">
         <v>7</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="44" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1671,8 +1679,8 @@
       <c r="Z16" s="23"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="48"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
@@ -1706,10 +1714,10 @@
       <c r="Z17" s="22"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="47">
+      <c r="A18" s="42">
         <v>8</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1747,8 +1755,8 @@
       <c r="Z18" s="23"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="48"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="7" t="s">
         <v>1</v>
       </c>
@@ -1782,10 +1790,10 @@
       <c r="Z19" s="22"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="47">
+      <c r="A20" s="42">
         <v>9</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="44" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1823,8 +1831,8 @@
       <c r="Z20" s="23"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="48"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1858,10 +1866,10 @@
       <c r="Z21" s="22"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="47">
+      <c r="A22" s="42">
         <v>10</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="44" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1903,8 +1911,8 @@
       <c r="Z22" s="36"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="48"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="7" t="s">
         <v>1</v>
       </c>
@@ -1938,10 +1946,10 @@
       <c r="Z23" s="22"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="47">
+      <c r="A24" s="42">
         <v>11</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="44" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1981,8 +1989,8 @@
       <c r="Z24" s="23"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="48"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="7" t="s">
         <v>1</v>
       </c>
@@ -2016,10 +2024,10 @@
       <c r="Z25" s="22"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="47">
+      <c r="A26" s="42">
         <v>12</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="44" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -2061,8 +2069,8 @@
       <c r="Z26" s="23"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="48"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="7" t="s">
         <v>1</v>
       </c>
@@ -2096,10 +2104,10 @@
       <c r="Z27" s="22"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="47">
+      <c r="A28" s="42">
         <v>13</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="44" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -2137,8 +2145,8 @@
       <c r="Z28" s="23"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="48"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="7" t="s">
         <v>1</v>
       </c>
@@ -2172,10 +2180,10 @@
       <c r="Z29" s="22"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="47">
+      <c r="A30" s="42">
         <v>14</v>
       </c>
-      <c r="B30" s="49"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
@@ -2207,8 +2215,8 @@
       <c r="Z30" s="23"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="48"/>
-      <c r="B31" s="50"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="7" t="s">
         <v>1</v>
       </c>
@@ -2240,10 +2248,10 @@
       <c r="Z31" s="22"/>
     </row>
     <row r="32" spans="1:26">
-      <c r="A32" s="47">
+      <c r="A32" s="42">
         <v>15</v>
       </c>
-      <c r="B32" s="49"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="6" t="s">
         <v>0</v>
       </c>
@@ -2275,8 +2283,8 @@
       <c r="Z32" s="23"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="48"/>
-      <c r="B33" s="50"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="7" t="s">
         <v>1</v>
       </c>
@@ -2308,10 +2316,10 @@
       <c r="Z33" s="22"/>
     </row>
     <row r="34" spans="1:26">
-      <c r="A34" s="47">
+      <c r="A34" s="42">
         <v>16</v>
       </c>
-      <c r="B34" s="49"/>
+      <c r="B34" s="44"/>
       <c r="C34" s="6" t="s">
         <v>0</v>
       </c>
@@ -2343,8 +2351,8 @@
       <c r="Z34" s="23"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="48"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="7" t="s">
         <v>1</v>
       </c>
@@ -2376,10 +2384,10 @@
       <c r="Z35" s="22"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="47">
+      <c r="A36" s="42">
         <v>17</v>
       </c>
-      <c r="B36" s="49"/>
+      <c r="B36" s="44"/>
       <c r="C36" s="6" t="s">
         <v>0</v>
       </c>
@@ -2411,8 +2419,8 @@
       <c r="Z36" s="23"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="48"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="7" t="s">
         <v>1</v>
       </c>
@@ -2444,10 +2452,10 @@
       <c r="Z37" s="22"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="47">
+      <c r="A38" s="42">
         <v>19</v>
       </c>
-      <c r="B38" s="49"/>
+      <c r="B38" s="44"/>
       <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
@@ -2479,8 +2487,8 @@
       <c r="Z38" s="23"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="48"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="45"/>
       <c r="C39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2512,10 +2520,10 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="47">
+      <c r="A40" s="42">
         <v>20</v>
       </c>
-      <c r="B40" s="49"/>
+      <c r="B40" s="44"/>
       <c r="C40" s="6" t="s">
         <v>0</v>
       </c>
@@ -2547,8 +2555,8 @@
       <c r="Z40" s="23"/>
     </row>
     <row r="41" spans="1:26">
-      <c r="A41" s="48"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="7" t="s">
         <v>1</v>
       </c>
@@ -2596,7 +2604,7 @@
       <c r="D43" s="10"/>
       <c r="E43" s="16">
         <f>E5+E7+E9+E11+E13+E15+E17+E19+E21+E23+E25+E27+E29+E31+E33+E35+E37+E39+E41</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="8:8">
@@ -2606,12 +2614,33 @@
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="41">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A34:A35"/>
@@ -2620,33 +2649,12 @@
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
   </mergeCells>
   <conditionalFormatting sqref="F40:Z40 F38:Z38 F36:Z36 F34:Z34 F32:Z32 F30:Z30 F28:Z28 F26:Z26 F22:Z22 F20:Z20 F18:Z18 F16:Z16 F14:Z14 F12:Z12 F10:Z10 F8:Z8 F6:Z6 F24:Z24 F4:Z4">
     <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="M">

</xml_diff>

<commit_message>
Schema überarbeitet, Pulsgen. angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -656,20 +656,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -684,6 +670,20 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,7 +1045,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J12" sqref="J12"/>
+      <selection pane="topRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
@@ -1061,13 +1061,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
@@ -1086,17 +1086,17 @@
     </row>
     <row r="2" spans="1:26" customFormat="1" ht="42" customHeight="1">
       <c r="C2" s="28"/>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="44" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" thickBot="1">
       <c r="C3" s="39"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="49"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="12">
         <v>44061</v>
       </c>
@@ -1150,10 +1150,10 @@
       <c r="Z3" s="38"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="42">
-        <v>1</v>
-      </c>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="47">
+        <v>1</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -1191,8 +1191,8 @@
       <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="43"/>
-      <c r="B5" s="45"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1228,10 +1228,10 @@
       <c r="Z5" s="22"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="42">
+      <c r="A6" s="47">
         <v>2</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1279,8 +1279,8 @@
       <c r="Z6" s="23"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="43"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1316,10 +1316,10 @@
       <c r="Z7" s="22"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="42">
+      <c r="A8" s="47">
         <v>3</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1363,8 +1363,8 @@
       <c r="Z8" s="23"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="43"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="E9" s="20">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F9" s="8">
         <v>1</v>
@@ -1386,9 +1386,15 @@
       <c r="J9" s="8">
         <v>1</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1</v>
+      </c>
+      <c r="M9" s="8">
+        <v>1</v>
+      </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
@@ -1404,10 +1410,10 @@
       <c r="Z9" s="22"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="42">
+      <c r="A10" s="47">
         <v>4</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="49" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1445,8 +1451,8 @@
       <c r="Z10" s="23"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="43"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1455,7 +1461,7 @@
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="8"/>
@@ -1466,9 +1472,15 @@
       <c r="J11" s="8">
         <v>1</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8">
+        <v>1</v>
+      </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
@@ -1484,10 +1496,10 @@
       <c r="Z11" s="22"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="42">
+      <c r="A12" s="47">
         <v>5</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1525,8 +1537,8 @@
       <c r="Z12" s="23"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="43"/>
-      <c r="B13" s="45"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1560,10 +1572,10 @@
       <c r="Z13" s="22"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="42">
+      <c r="A14" s="47">
         <v>6</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="49" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1601,8 +1613,8 @@
       <c r="Z14" s="23"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="43"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1636,10 +1648,10 @@
       <c r="Z15" s="22"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="42">
+      <c r="A16" s="47">
         <v>7</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="49" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1679,8 +1691,8 @@
       <c r="Z16" s="23"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="43"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
@@ -1714,10 +1726,10 @@
       <c r="Z17" s="22"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="42">
+      <c r="A18" s="47">
         <v>8</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="49" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1755,8 +1767,8 @@
       <c r="Z18" s="23"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="43"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="7" t="s">
         <v>1</v>
       </c>
@@ -1790,10 +1802,10 @@
       <c r="Z19" s="22"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="42">
+      <c r="A20" s="47">
         <v>9</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="49" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1831,8 +1843,8 @@
       <c r="Z20" s="23"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="43"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1866,10 +1878,10 @@
       <c r="Z21" s="22"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="42">
+      <c r="A22" s="47">
         <v>10</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="49" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1911,8 +1923,8 @@
       <c r="Z22" s="36"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="43"/>
-      <c r="B23" s="45"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="7" t="s">
         <v>1</v>
       </c>
@@ -1946,10 +1958,10 @@
       <c r="Z23" s="22"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="42">
+      <c r="A24" s="47">
         <v>11</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="49" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1989,8 +2001,8 @@
       <c r="Z24" s="23"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="43"/>
-      <c r="B25" s="45"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="7" t="s">
         <v>1</v>
       </c>
@@ -2024,10 +2036,10 @@
       <c r="Z25" s="22"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="42">
+      <c r="A26" s="47">
         <v>12</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="49" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -2069,8 +2081,8 @@
       <c r="Z26" s="23"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="43"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="7" t="s">
         <v>1</v>
       </c>
@@ -2104,10 +2116,10 @@
       <c r="Z27" s="22"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="42">
+      <c r="A28" s="47">
         <v>13</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="49" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -2145,8 +2157,8 @@
       <c r="Z28" s="23"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="43"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="7" t="s">
         <v>1</v>
       </c>
@@ -2180,10 +2192,10 @@
       <c r="Z29" s="22"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="42">
+      <c r="A30" s="47">
         <v>14</v>
       </c>
-      <c r="B30" s="44"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
@@ -2215,8 +2227,8 @@
       <c r="Z30" s="23"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="43"/>
-      <c r="B31" s="45"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="7" t="s">
         <v>1</v>
       </c>
@@ -2248,10 +2260,10 @@
       <c r="Z31" s="22"/>
     </row>
     <row r="32" spans="1:26">
-      <c r="A32" s="42">
+      <c r="A32" s="47">
         <v>15</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="6" t="s">
         <v>0</v>
       </c>
@@ -2283,8 +2295,8 @@
       <c r="Z32" s="23"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="43"/>
-      <c r="B33" s="45"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="50"/>
       <c r="C33" s="7" t="s">
         <v>1</v>
       </c>
@@ -2316,10 +2328,10 @@
       <c r="Z33" s="22"/>
     </row>
     <row r="34" spans="1:26">
-      <c r="A34" s="42">
+      <c r="A34" s="47">
         <v>16</v>
       </c>
-      <c r="B34" s="44"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="6" t="s">
         <v>0</v>
       </c>
@@ -2351,8 +2363,8 @@
       <c r="Z34" s="23"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="43"/>
-      <c r="B35" s="45"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="7" t="s">
         <v>1</v>
       </c>
@@ -2384,10 +2396,10 @@
       <c r="Z35" s="22"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="42">
+      <c r="A36" s="47">
         <v>17</v>
       </c>
-      <c r="B36" s="44"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="6" t="s">
         <v>0</v>
       </c>
@@ -2419,8 +2431,8 @@
       <c r="Z36" s="23"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="43"/>
-      <c r="B37" s="45"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="7" t="s">
         <v>1</v>
       </c>
@@ -2452,10 +2464,10 @@
       <c r="Z37" s="22"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="42">
+      <c r="A38" s="47">
         <v>19</v>
       </c>
-      <c r="B38" s="44"/>
+      <c r="B38" s="49"/>
       <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
@@ -2487,8 +2499,8 @@
       <c r="Z38" s="23"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="43"/>
-      <c r="B39" s="45"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2520,10 +2532,10 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="42">
+      <c r="A40" s="47">
         <v>20</v>
       </c>
-      <c r="B40" s="44"/>
+      <c r="B40" s="49"/>
       <c r="C40" s="6" t="s">
         <v>0</v>
       </c>
@@ -2555,8 +2567,8 @@
       <c r="Z40" s="23"/>
     </row>
     <row r="41" spans="1:26">
-      <c r="A41" s="43"/>
-      <c r="B41" s="45"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="7" t="s">
         <v>1</v>
       </c>
@@ -2604,7 +2616,7 @@
       <c r="D43" s="10"/>
       <c r="E43" s="16">
         <f>E5+E7+E9+E11+E13+E15+E17+E19+E21+E23+E25+E27+E29+E31+E33+E35+E37+E39+E41</f>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="8:8">
@@ -2614,33 +2626,12 @@
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="41">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A34:A35"/>
@@ -2649,12 +2640,33 @@
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F40:Z40 F38:Z38 F36:Z36 F34:Z34 F32:Z32 F30:Z30 F28:Z28 F26:Z26 F22:Z22 F20:Z20 F18:Z18 F16:Z16 F14:Z14 F12:Z12 F10:Z10 F8:Z8 F6:Z6 F24:Z24 F4:Z4">
     <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="M">

</xml_diff>